<commit_message>
Fix: Crawling Tread 10 +
쓰레드 10개로 구성 및 소박스 대박스 분류
</commit_message>
<xml_diff>
--- a/data_bacode.xlsx
+++ b/data_bacode.xlsx
@@ -481,7 +481,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B16533"/>
+  <dimension ref="A1:E16533"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A514" workbookViewId="0">
       <selection activeCell="E520" sqref="E520"/>
@@ -503,220 +503,805 @@
       <c r="A2" s="2" t="n">
         <v>1472225646</v>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" t="n">
+        <v>1472225646</v>
+      </c>
+      <c r="C2" t="inlineStr">
         <is>
           <t>8809624601295</t>
         </is>
       </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>정보 없음</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>정보 없음</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
         <v>1472225647</v>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B3" t="n">
+        <v>1472225647</v>
+      </c>
+      <c r="C3" t="inlineStr">
         <is>
           <t>8809624601301</t>
         </is>
       </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>정보 없음</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>정보 없음</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
         <v>1472225648</v>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B4" t="n">
+        <v>1472225648</v>
+      </c>
+      <c r="C4" t="inlineStr">
         <is>
           <t>8809633572845</t>
         </is>
       </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>정보 없음</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>정보 없음</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
         <v>1472225649</v>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B5" t="n">
+        <v>1472225649</v>
+      </c>
+      <c r="C5" t="inlineStr">
         <is>
           <t>8809675219395</t>
         </is>
       </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>정보 없음</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>정보 없음</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
         <v>1472225650</v>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B6" t="n">
+        <v>1472225650</v>
+      </c>
+      <c r="C6" t="inlineStr">
         <is>
           <t>8809727613577</t>
         </is>
       </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>정보 없음</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>정보 없음</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
         <v>1472225651</v>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="B7" t="n">
+        <v>1472225651</v>
+      </c>
+      <c r="C7" t="inlineStr">
         <is>
           <t>8809727618831</t>
         </is>
       </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>정보 없음</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>정보 없음</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
         <v>1472225652</v>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="B8" t="n">
+        <v>1472225652</v>
+      </c>
+      <c r="C8" t="inlineStr">
         <is>
           <t>8809781561548</t>
         </is>
       </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>정보 없음</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>정보 없음</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
         <v>1472225653</v>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B9" t="n">
+        <v>1472225653</v>
+      </c>
+      <c r="C9" t="inlineStr">
         <is>
           <t>8809781568240</t>
         </is>
       </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>정보 없음</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>정보 없음</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="n">
         <v>1472225654</v>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="B10" t="n">
+        <v>1472225654</v>
+      </c>
+      <c r="C10" t="inlineStr">
         <is>
           <t>8809781568257</t>
         </is>
       </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>정보 없음</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>정보 없음</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="n">
         <v>1472225655</v>
       </c>
+      <c r="B11" t="n">
+        <v>1472225655</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>8809885085445</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>정보 없음</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>정보 없음</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="n">
         <v>1472225656</v>
       </c>
+      <c r="B12" t="n">
+        <v>1472225656</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>8809885085452</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>정보 없음</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>정보 없음</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="n">
         <v>1472225657</v>
       </c>
+      <c r="B13" t="n">
+        <v>1472225657</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>8809885085469</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>정보 없음</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>정보 없음</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="n">
         <v>1472225658</v>
       </c>
+      <c r="B14" t="n">
+        <v>1472225658</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>8809885085476</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>정보 없음</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>정보 없음</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="2" t="n">
         <v>1472225659</v>
       </c>
+      <c r="B15" t="n">
+        <v>1472225659</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>8809885085483</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>정보 없음</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>정보 없음</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="2" t="n">
         <v>1472225628</v>
       </c>
+      <c r="B16" t="n">
+        <v>1472225628</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>8809885085803</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>정보 없음</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>정보 없음</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="2" t="n">
         <v>1472225629</v>
       </c>
+      <c r="B17" t="n">
+        <v>1472225629</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>8809885085858</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>정보 없음</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>정보 없음</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="2" t="n">
         <v>1472225630</v>
       </c>
+      <c r="B18" t="n">
+        <v>1472225630</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>8809885085810</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>정보 없음</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>정보 없음</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="n">
         <v>1472225631</v>
       </c>
+      <c r="B19" t="n">
+        <v>1472225631</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>8809885085865</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>정보 없음</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>정보 없음</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="n">
         <v>1472225632</v>
       </c>
+      <c r="B20" t="n">
+        <v>1472225632</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>8809885085827</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>정보 없음</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>정보 없음</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="n">
         <v>1472225633</v>
       </c>
+      <c r="B21" t="n">
+        <v>1472225633</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>8809885085964</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>정보 없음</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>정보 없음</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="n">
         <v>1472225634</v>
       </c>
+      <c r="B22" t="n">
+        <v>1472225634</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>8809885085872</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>정보 없음</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>정보 없음</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="2" t="n">
         <v>1472225635</v>
       </c>
+      <c r="B23" t="n">
+        <v>1472225635</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>8809885085971</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>정보 없음</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>정보 없음</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="n">
         <v>1472225636</v>
       </c>
+      <c r="B24" t="n">
+        <v>1472225636</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>8809885085896</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>정보 없음</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>정보 없음</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="n">
         <v>1472225637</v>
       </c>
+      <c r="B25" t="n">
+        <v>1472225637</v>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>8809885085940</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>정보 없음</t>
+        </is>
+      </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>정보 없음</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="n">
         <v>1472225638</v>
       </c>
+      <c r="B26" t="n">
+        <v>1472225638</v>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>8809885085902</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>정보 없음</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>정보 없음</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="n">
         <v>1472225639</v>
       </c>
+      <c r="B27" t="n">
+        <v>1472225639</v>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>8809885085834</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>정보 없음</t>
+        </is>
+      </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>정보 없음</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="n">
         <v>1472225640</v>
       </c>
+      <c r="B28" t="n">
+        <v>1472225640</v>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>8809885085957</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>정보 없음</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>정보 없음</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="n">
         <v>1472225641</v>
       </c>
+      <c r="B29" t="n">
+        <v>1472225641</v>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>8809885085919</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>정보 없음</t>
+        </is>
+      </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>정보 없음</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" s="2" t="n">
         <v>1472225642</v>
       </c>
+      <c r="B30" t="n">
+        <v>1472225642</v>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>8809885085889</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>정보 없음</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>정보 없음</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" s="2" t="n">
         <v>1472225643</v>
       </c>
+      <c r="B31" t="n">
+        <v>1472225643</v>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>8809885085926</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>정보 없음</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>정보 없음</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="n">
         <v>1472225644</v>
       </c>
+      <c r="B32" t="n">
+        <v>1472225644</v>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>8809885085841</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>정보 없음</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>정보 없음</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="n">
         <v>1472225645</v>
       </c>
+      <c r="B33" t="n">
+        <v>1472225645</v>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>8809885085933</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>정보 없음</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>정보 없음</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" s="2" t="n">
         <v>1472225623</v>
       </c>
+      <c r="B34" t="n">
+        <v>1472225623</v>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>8809656959241</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>정보 없음</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>정보 없음</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" s="2" t="n">
         <v>1472225624</v>
       </c>
+      <c r="B35" t="n">
+        <v>1472225624</v>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>8809379550053</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>정보 없음</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" s="2" t="n">
         <v>1472225625</v>
+      </c>
+      <c r="B36" t="n">
+        <v>1472225625</v>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>8809379550008</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>정보 없음</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
       </c>
     </row>
     <row r="37">

</xml_diff>